<commit_message>
Huge debug session and experimenting with Ruurd
</commit_message>
<xml_diff>
--- a/Data/OneScenario/Instance_storage_costs_option3.xlsx
+++ b/Data/OneScenario/Instance_storage_costs_option3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/OneScenario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C056E96A-4F4E-DE45-9833-1B28D7804B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2170F975-BE6B-C04B-AC8B-39CBA2FAF302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="4100" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="9" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualisation" sheetId="7" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="346">
   <si>
     <t>ID</t>
   </si>
@@ -1149,6 +1149,9 @@
   <si>
     <t>Increase storage costs stage 3</t>
   </si>
+  <si>
+    <t>Length</t>
+  </si>
 </sst>
 </file>
 
@@ -1512,7 +1515,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
@@ -1608,6 +1611,15 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1620,15 +1632,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
@@ -2135,10 +2140,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2902688A-D2A3-854F-B341-C0BEC53AF991}">
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2159,7 +2164,7 @@
     <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2211,8 +2216,11 @@
       <c r="Q1" s="54" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S1" s="69" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2254,10 +2262,12 @@
         <v>7</v>
       </c>
       <c r="M2" s="2">
-        <v>1E-3</v>
+        <f>S2</f>
+        <v>0.01</v>
       </c>
       <c r="N2" s="3">
-        <v>1E-3</v>
+        <f>S2</f>
+        <v>0.01</v>
       </c>
       <c r="O2" t="str" cm="1">
         <f t="array" ref="O2">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K2,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K2,5), ",",".")</f>
@@ -2271,8 +2281,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K2,4), INDEX(Nodes!$A$3:$E$64,Arcs!L2,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K2,5), INDEX(Nodes!$A$3:$E$64,Arcs!L2,5)), ",", ".")</f>
         <v>2.96794024746388 60.5519809989487</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2314,10 +2327,12 @@
         <v>14</v>
       </c>
       <c r="M3" s="2">
-        <v>1E-3</v>
+        <f t="shared" ref="M3:M62" si="2">S3</f>
+        <v>0.01</v>
       </c>
       <c r="N3" s="3">
-        <v>1E-3</v>
+        <f t="shared" ref="N3:N62" si="3">S3</f>
+        <v>0.01</v>
       </c>
       <c r="O3" t="str" cm="1">
         <f t="array" ref="O3">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K3,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K3,5), ",",".")</f>
@@ -2331,8 +2346,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K3,4), INDEX(Nodes!$A$3:$E$64,Arcs!L3,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K3,5), INDEX(Nodes!$A$3:$E$64,Arcs!L3,5)), ",", ".")</f>
         <v>7.11614205264601 64.2919112956052</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2374,10 +2392,12 @@
         <v>36</v>
       </c>
       <c r="M4" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.70699999999999996</v>
       </c>
       <c r="N4" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.70699999999999996</v>
       </c>
       <c r="O4" t="str" cm="1">
         <f t="array" ref="O4">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K4,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K4,5), ",",".")</f>
@@ -2391,8 +2411,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K4,4), INDEX(Nodes!$A$3:$E$64,Arcs!L4,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K4,5), INDEX(Nodes!$A$3:$E$64,Arcs!L4,5)), ",", ".")</f>
         <v>5.10073123031673 60.7874221331929</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S4">
+        <v>0.70699999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2434,10 +2457,12 @@
         <v>23</v>
       </c>
       <c r="M5" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.4002</v>
       </c>
       <c r="N5" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.4002</v>
       </c>
       <c r="O5" t="str" cm="1">
         <f t="array" ref="O5">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K5,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K5,5), ",",".")</f>
@@ -2451,8 +2476,12 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K5,4), INDEX(Nodes!$A$3:$E$64,Arcs!L5,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K5,5), INDEX(Nodes!$A$3:$E$64,Arcs!L5,5)), ",", ".")</f>
         <v>3.34351308302685 56.9475590087063</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S5">
+        <f>0.667*0.6</f>
+        <v>0.4002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2494,10 +2523,12 @@
         <v>21</v>
       </c>
       <c r="M6" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.26680000000000004</v>
       </c>
       <c r="N6" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.26680000000000004</v>
       </c>
       <c r="O6" t="str" cm="1">
         <f t="array" ref="O6">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K6,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K6,5), ",",".")</f>
@@ -2511,8 +2542,12 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K6,4), INDEX(Nodes!$A$3:$E$64,Arcs!L6,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K6,5), INDEX(Nodes!$A$3:$E$64,Arcs!L6,5)), ",", ".")</f>
         <v>5.77452100000005 54.6933345000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S6">
+        <f>0.667*0.4</f>
+        <v>0.26680000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2554,10 +2589,12 @@
         <v>5</v>
       </c>
       <c r="M7" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.44</v>
       </c>
       <c r="N7" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.44</v>
       </c>
       <c r="O7" t="str" cm="1">
         <f t="array" ref="O7">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K7,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K7,5), ",",".")</f>
@@ -2571,8 +2608,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K7,4), INDEX(Nodes!$A$3:$E$64,Arcs!L7,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K7,5), INDEX(Nodes!$A$3:$E$64,Arcs!L7,5)), ",", ".")</f>
         <v>6.00836066672178 57.4910578139182</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S7">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2614,10 +2654,12 @@
         <v>21</v>
       </c>
       <c r="M8" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.22</v>
       </c>
       <c r="N8" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.22</v>
       </c>
       <c r="O8" t="str" cm="1">
         <f t="array" ref="O8">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K8,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K8,5), ",",".")</f>
@@ -2631,8 +2673,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K8,4), INDEX(Nodes!$A$3:$E$64,Arcs!L8,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K8,5), INDEX(Nodes!$A$3:$E$64,Arcs!L8,5)), ",", ".")</f>
         <v>6.91511000000002 54.69485</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S8">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2658,7 +2703,7 @@
         <f t="shared" si="1"/>
         <v>LINESTRING(2.46440416605363 58.1881490174125,2.35855658302684 54.6172775087063,2.25270900000004 51.046406)</v>
       </c>
-      <c r="I9" s="42">
+      <c r="I9" s="68">
         <v>54.2</v>
       </c>
       <c r="J9" s="1" t="str">
@@ -2674,10 +2719,12 @@
         <v>17</v>
       </c>
       <c r="M9" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.84</v>
       </c>
       <c r="N9" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.84</v>
       </c>
       <c r="O9" t="str" cm="1">
         <f t="array" ref="O9">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K9,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K9,5), ",",".")</f>
@@ -2691,8 +2738,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K9,4), INDEX(Nodes!$A$3:$E$64,Arcs!L9,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K9,5), INDEX(Nodes!$A$3:$E$64,Arcs!L9,5)), ",", ".")</f>
         <v>2.35855658302684 54.6172775087063</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S9">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2734,10 +2784,12 @@
         <v>37</v>
       </c>
       <c r="M10" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.14699999999999999</v>
       </c>
       <c r="N10" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.14699999999999999</v>
       </c>
       <c r="O10" t="str" cm="1">
         <f t="array" ref="O10">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K10,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K10,5), ",",".")</f>
@@ -2751,8 +2803,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K10,4), INDEX(Nodes!$A$3:$E$64,Arcs!L10,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K10,5), INDEX(Nodes!$A$3:$E$64,Arcs!L10,5)), ",", ".")</f>
         <v>3.67283754339515 60.8114652109992</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S10">
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2794,10 +2849,12 @@
         <v>51</v>
       </c>
       <c r="M11" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.627</v>
       </c>
       <c r="N11" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.627</v>
       </c>
       <c r="O11" t="str" cm="1">
         <f t="array" ref="O11">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K11,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K11,5), ",",".")</f>
@@ -2811,8 +2868,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K11,4), INDEX(Nodes!$A$3:$E$64,Arcs!L11,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K11,5), INDEX(Nodes!$A$3:$E$64,Arcs!L11,5)), ",", ".")</f>
         <v>4.43081880699815 60.6082514294188</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S11">
+        <v>0.627</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2854,10 +2914,12 @@
         <v>18</v>
       </c>
       <c r="M12" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.54300000000000004</v>
       </c>
       <c r="N12" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.54300000000000004</v>
       </c>
       <c r="O12" t="str" cm="1">
         <f t="array" ref="O12">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K12,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K12,5), ",",".")</f>
@@ -2871,8 +2933,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K12,4), INDEX(Nodes!$A$3:$E$64,Arcs!L12,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K12,5), INDEX(Nodes!$A$3:$E$64,Arcs!L12,5)), ",", ".")</f>
         <v>1.01594869849812 56.0120875869188</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S12">
+        <v>0.54300000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2914,10 +2979,12 @@
         <v>42</v>
       </c>
       <c r="M13" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.128</v>
       </c>
       <c r="N13" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.128</v>
       </c>
       <c r="O13" t="str" cm="1">
         <f t="array" ref="O13">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K13,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K13,5), ",",".")</f>
@@ -2931,8 +2998,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K13,4), INDEX(Nodes!$A$3:$E$64,Arcs!L13,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K13,5), INDEX(Nodes!$A$3:$E$64,Arcs!L13,5)), ",", ".")</f>
         <v>7.44000255895174 65.5569234497045</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S13">
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2974,10 +3044,12 @@
         <v>20</v>
       </c>
       <c r="M14" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.02</v>
       </c>
       <c r="N14" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.02</v>
       </c>
       <c r="O14" t="str" cm="1">
         <f t="array" ref="O14">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K14,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K14,5), ",",".")</f>
@@ -2991,8 +3063,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K14,4), INDEX(Nodes!$A$3:$E$64,Arcs!L14,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K14,5), INDEX(Nodes!$A$3:$E$64,Arcs!L14,5)), ",", ".")</f>
         <v>3.28025150000001 56.5201845</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S14">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3034,10 +3109,12 @@
         <v>4</v>
       </c>
       <c r="M15" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.14366666666666666</v>
       </c>
       <c r="N15" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.14366666666666666</v>
       </c>
       <c r="O15" t="str" cm="1">
         <f t="array" ref="O15">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K15,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K15,5), ",",".")</f>
@@ -3051,8 +3128,12 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K15,4), INDEX(Nodes!$A$3:$E$64,Arcs!L15,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K15,5), INDEX(Nodes!$A$3:$E$64,Arcs!L15,5)), ",", ".")</f>
         <v>3.94372505908058 55.9746756858192</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S15">
+        <f>0.431/3</f>
+        <v>0.14366666666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3094,10 +3175,12 @@
         <v>30</v>
       </c>
       <c r="M16" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.14366666666666666</v>
       </c>
       <c r="N16" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.14366666666666666</v>
       </c>
       <c r="O16" t="str" cm="1">
         <f t="array" ref="O16">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K16,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K16,5), ",",".")</f>
@@ -3111,8 +3194,12 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K16,4), INDEX(Nodes!$A$3:$E$64,Arcs!L16,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K16,5), INDEX(Nodes!$A$3:$E$64,Arcs!L16,5)), ",", ".")</f>
         <v>5.2987903360241 54.982391852912</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S16">
+        <f>0.431/3</f>
+        <v>0.14366666666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3154,10 +3241,12 @@
         <v>22</v>
       </c>
       <c r="M17" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.14366666666666666</v>
       </c>
       <c r="N17" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.14366666666666666</v>
       </c>
       <c r="O17" t="str" cm="1">
         <f t="array" ref="O17">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K17,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K17,5), ",",".")</f>
@@ -3171,8 +3260,12 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K17,4), INDEX(Nodes!$A$3:$E$64,Arcs!L17,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K17,5), INDEX(Nodes!$A$3:$E$64,Arcs!L17,5)), ",", ".")</f>
         <v>6.61496177694355 53.9260006670928</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S17">
+        <f>0.431/3</f>
+        <v>0.14366666666666666</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3214,10 +3307,12 @@
         <v>33</v>
       </c>
       <c r="M18" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.109</v>
       </c>
       <c r="N18" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.109</v>
       </c>
       <c r="O18" t="str" cm="1">
         <f t="array" ref="O18">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K18,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K18,5), ",",".")</f>
@@ -3231,8 +3326,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K18,4), INDEX(Nodes!$A$3:$E$64,Arcs!L18,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K18,5), INDEX(Nodes!$A$3:$E$64,Arcs!L18,5)), ",", ".")</f>
         <v>2.52963583723616 60.0289879024106</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S18">
+        <v>0.109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3274,10 +3372,12 @@
         <v>36</v>
       </c>
       <c r="M19" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.153</v>
       </c>
       <c r="N19" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.153</v>
       </c>
       <c r="O19" t="str" cm="1">
         <f t="array" ref="O19">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K19,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K19,5), ",",".")</f>
@@ -3291,8 +3391,12 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K19,4), INDEX(Nodes!$A$3:$E$64,Arcs!L19,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K19,5), INDEX(Nodes!$A$3:$E$64,Arcs!L19,5)), ",", ".")</f>
         <v>3.67942866672181 60.2289728139182</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S19">
+        <f>0.306/2</f>
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3334,10 +3438,12 @@
         <v>16</v>
       </c>
       <c r="M20" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.155</v>
       </c>
       <c r="N20" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.155</v>
       </c>
       <c r="O20" t="str" cm="1">
         <f t="array" ref="O20">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K20,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K20,5), ",",".")</f>
@@ -3351,8 +3457,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K20,4), INDEX(Nodes!$A$3:$E$64,Arcs!L20,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K20,5), INDEX(Nodes!$A$3:$E$64,Arcs!L20,5)), ",", ".")</f>
         <v>2.35412777628591 58.8775735508799</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S20">
+        <v>0.155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3394,10 +3503,12 @@
         <v>16</v>
       </c>
       <c r="M21" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.22800000000000001</v>
       </c>
       <c r="N21" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.22800000000000001</v>
       </c>
       <c r="O21" t="str" cm="1">
         <f t="array" ref="O21">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K21,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K21,5), ",",".")</f>
@@ -3411,8 +3522,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K21,4), INDEX(Nodes!$A$3:$E$64,Arcs!L21,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K21,5), INDEX(Nodes!$A$3:$E$64,Arcs!L21,5)), ",", ".")</f>
         <v>3.99332715402322 58.7282624284256</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S21">
+        <v>0.22800000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3454,10 +3568,12 @@
         <v>43</v>
       </c>
       <c r="M22" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.20300000000000001</v>
       </c>
       <c r="N22" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.20300000000000001</v>
       </c>
       <c r="O22" t="str" cm="1">
         <f t="array" ref="O22">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K22,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K22,5), ",",".")</f>
@@ -3471,8 +3587,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K22,4), INDEX(Nodes!$A$3:$E$64,Arcs!L22,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K22,5), INDEX(Nodes!$A$3:$E$64,Arcs!L22,5)), ",", ".")</f>
         <v>2.90211798730145 57.3373891145074</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S22">
+        <v>0.20300000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3514,10 +3633,12 @@
         <v>53</v>
       </c>
       <c r="M23" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.153</v>
       </c>
       <c r="N23" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.153</v>
       </c>
       <c r="O23" t="str" cm="1">
         <f t="array" ref="O23">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K23,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K23,5), ",",".")</f>
@@ -3531,8 +3652,12 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K23,4), INDEX(Nodes!$A$3:$E$64,Arcs!L23,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K23,5), INDEX(Nodes!$A$3:$E$64,Arcs!L23,5)), ",", ".")</f>
         <v>1.83873088879207 61.1941375238008</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S23">
+        <f>0.306/2</f>
+        <v>0.153</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3574,10 +3699,12 @@
         <v>24</v>
       </c>
       <c r="M24" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>2.3E-2</v>
       </c>
       <c r="N24" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>2.3E-2</v>
       </c>
       <c r="O24" t="str" cm="1">
         <f t="array" ref="O24">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K24,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K24,5), ",",".")</f>
@@ -3591,8 +3718,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K24,4), INDEX(Nodes!$A$3:$E$64,Arcs!L24,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K24,5), INDEX(Nodes!$A$3:$E$64,Arcs!L24,5)), ",", ".")</f>
         <v>1.76585744579207 61.1122317403008</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S24">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3634,10 +3764,12 @@
         <v>52</v>
       </c>
       <c r="M25" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.36099999999999999</v>
       </c>
       <c r="N25" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.36099999999999999</v>
       </c>
       <c r="O25" t="str" cm="1">
         <f t="array" ref="O25">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K25,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K25,5), ",",".")</f>
@@ -3651,8 +3783,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K25,4), INDEX(Nodes!$A$3:$E$64,Arcs!L25,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K25,5), INDEX(Nodes!$A$3:$E$64,Arcs!L25,5)), ",", ".")</f>
         <v>0.204787243746546 58.5755231756066</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S25">
+        <v>0.36099999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3678,7 +3813,7 @@
         <f t="shared" si="1"/>
         <v>LINESTRING(1.91586639699623 58.3649441738375,2.60784119849812 56.5772190869188,3.29981600000002 54.789494)</v>
       </c>
-      <c r="I26" s="42">
+      <c r="I26" s="68">
         <v>42.2</v>
       </c>
       <c r="J26" s="1" t="str">
@@ -3694,10 +3829,12 @@
         <v>59</v>
       </c>
       <c r="M26" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.40649999999999997</v>
       </c>
       <c r="N26" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.40649999999999997</v>
       </c>
       <c r="O26" t="str" cm="1">
         <f t="array" ref="O26">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K26,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K26,5), ",",".")</f>
@@ -3711,8 +3848,12 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K26,4), INDEX(Nodes!$A$3:$E$64,Arcs!L26,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K26,5), INDEX(Nodes!$A$3:$E$64,Arcs!L26,5)), ",", ".")</f>
         <v>2.60784119849812 56.5772190869188</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S26">
+        <f>0.813/2</f>
+        <v>0.40649999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3738,7 +3879,7 @@
         <f t="shared" si="1"/>
         <v>LINESTRING(3.29981600000002 54.789494,3.26480650000005 53.070001,3.22979700000008 51.350508)</v>
       </c>
-      <c r="I27" s="42">
+      <c r="I27" s="68">
         <v>42.2</v>
       </c>
       <c r="J27" s="1" t="str">
@@ -3754,10 +3895,12 @@
         <v>58</v>
       </c>
       <c r="M27" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.40649999999999997</v>
       </c>
       <c r="N27" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.40649999999999997</v>
       </c>
       <c r="O27" t="str" cm="1">
         <f t="array" ref="O27">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K27,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K27,5), ",",".")</f>
@@ -3771,8 +3914,12 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K27,4), INDEX(Nodes!$A$3:$E$64,Arcs!L27,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K27,5), INDEX(Nodes!$A$3:$E$64,Arcs!L27,5)), ",", ".")</f>
         <v>3.26480650000005 53.070001</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S27">
+        <f>0.813/2</f>
+        <v>0.40649999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3814,10 +3961,12 @@
         <v>51</v>
       </c>
       <c r="M28" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.29899999999999999</v>
       </c>
       <c r="N28" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.29899999999999999</v>
       </c>
       <c r="O28" t="str" cm="1">
         <f t="array" ref="O28">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K28,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K28,5), ",",".")</f>
@@ -3831,8 +3980,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K28,4), INDEX(Nodes!$A$3:$E$64,Arcs!L28,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K28,5), INDEX(Nodes!$A$3:$E$64,Arcs!L28,5)), ",", ".")</f>
         <v>3.37723170018861 59.455146330101</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S28">
+        <v>0.29899999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3874,10 +4026,12 @@
         <v>15</v>
       </c>
       <c r="M29" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.3</v>
       </c>
       <c r="N29" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.3</v>
       </c>
       <c r="O29" t="str" cm="1">
         <f t="array" ref="O29">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K29,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K29,5), ",",".")</f>
@@ -3891,8 +4045,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K29,4), INDEX(Nodes!$A$3:$E$64,Arcs!L29,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K29,5), INDEX(Nodes!$A$3:$E$64,Arcs!L29,5)), ",", ".")</f>
         <v>3.65150058471732 59.3667487518886</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S29">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3934,10 +4091,12 @@
         <v>27</v>
       </c>
       <c r="M30" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.13100000000000001</v>
       </c>
       <c r="N30" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.13100000000000001</v>
       </c>
       <c r="O30" t="str" cm="1">
         <f t="array" ref="O30">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K30,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K30,5), ",",".")</f>
@@ -3951,8 +4110,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K30,4), INDEX(Nodes!$A$3:$E$64,Arcs!L30,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K30,5), INDEX(Nodes!$A$3:$E$64,Arcs!L30,5)), ",", ".")</f>
         <v>2.80248752933371 61.1754957531437</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S30">
+        <v>0.13100000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3994,10 +4156,12 @@
         <v>28</v>
       </c>
       <c r="M31" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.02</v>
       </c>
       <c r="N31" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.02</v>
       </c>
       <c r="O31" t="str" cm="1">
         <f t="array" ref="O31">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K31,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K31,5), ",",".")</f>
@@ -4011,8 +4175,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K31,4), INDEX(Nodes!$A$3:$E$64,Arcs!L31,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K31,5), INDEX(Nodes!$A$3:$E$64,Arcs!L31,5)), ",", ".")</f>
         <v>2.36128039402701 59.3704008474222</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S31">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -4054,10 +4221,12 @@
         <v>50</v>
       </c>
       <c r="M32" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.05</v>
       </c>
       <c r="N32" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.05</v>
       </c>
       <c r="O32" t="str" cm="1">
         <f t="array" ref="O32">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K32,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K32,5), ",",".")</f>
@@ -4071,8 +4240,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K32,4), INDEX(Nodes!$A$3:$E$64,Arcs!L32,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K32,5), INDEX(Nodes!$A$3:$E$64,Arcs!L32,5)), ",", ".")</f>
         <v>1.82461800400345 58.6064721852943</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S32">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -4114,10 +4286,12 @@
         <v>56</v>
       </c>
       <c r="M33" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.25</v>
       </c>
       <c r="N33" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.25</v>
       </c>
       <c r="O33" t="str" cm="1">
         <f t="array" ref="O33">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K33,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K33,5), ",",".")</f>
@@ -4131,8 +4305,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K33,4), INDEX(Nodes!$A$3:$E$64,Arcs!L33,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K33,5), INDEX(Nodes!$A$3:$E$64,Arcs!L33,5)), ",", ".")</f>
         <v>7.98923048166803 64.3601952705966</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S33">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -4174,10 +4351,12 @@
         <v>42</v>
       </c>
       <c r="M34" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.01</v>
       </c>
       <c r="N34" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.01</v>
       </c>
       <c r="O34" t="str" cm="1">
         <f t="array" ref="O34">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K34,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K34,5), ",",".")</f>
@@ -4191,8 +4370,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K34,4), INDEX(Nodes!$A$3:$E$64,Arcs!L34,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K34,5), INDEX(Nodes!$A$3:$E$64,Arcs!L34,5)), ",", ".")</f>
         <v>7.0608532119336 65.2030077893163</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S34">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -4234,10 +4416,12 @@
         <v>35</v>
       </c>
       <c r="M35" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.01</v>
       </c>
       <c r="N35" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.01</v>
       </c>
       <c r="O35" t="str" cm="1">
         <f t="array" ref="O35">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K35,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K35,5), ",",".")</f>
@@ -4251,8 +4435,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K35,4), INDEX(Nodes!$A$3:$E$64,Arcs!L35,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K35,5), INDEX(Nodes!$A$3:$E$64,Arcs!L35,5)), ",", ".")</f>
         <v>3.80597375650467 59.0843695361675</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S35">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -4294,10 +4481,12 @@
         <v>25</v>
       </c>
       <c r="M36" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.01</v>
       </c>
       <c r="N36" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.01</v>
       </c>
       <c r="O36" t="str" cm="1">
         <f t="array" ref="O36">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K36,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K36,5), ",",".")</f>
@@ -4311,8 +4500,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K36,4), INDEX(Nodes!$A$3:$E$64,Arcs!L36,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K36,5), INDEX(Nodes!$A$3:$E$64,Arcs!L36,5)), ",", ".")</f>
         <v>2.01445157351417 60.1984986400223</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S36">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -4354,10 +4546,12 @@
         <v>44</v>
       </c>
       <c r="M37" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="N37" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.1</v>
       </c>
       <c r="O37" t="str" cm="1">
         <f t="array" ref="O37">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K37,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K37,5), ",",".")</f>
@@ -4371,8 +4565,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K37,4), INDEX(Nodes!$A$3:$E$64,Arcs!L37,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K37,5), INDEX(Nodes!$A$3:$E$64,Arcs!L37,5)), ",", ".")</f>
         <v>6.16626739450007 63.1898201775001</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S37">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -4414,10 +4611,12 @@
         <v>44</v>
       </c>
       <c r="M38" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.48199999999999998</v>
       </c>
       <c r="N38" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.48199999999999998</v>
       </c>
       <c r="O38" t="str" cm="1">
         <f t="array" ref="O38">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K38,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K38,5), ",",".")</f>
@@ -4431,8 +4630,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K38,4), INDEX(Nodes!$A$3:$E$64,Arcs!L38,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K38,5), INDEX(Nodes!$A$3:$E$64,Arcs!L38,5)), ",", ".")</f>
         <v>7.02649910850005 64.9535843425001</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S38">
+        <v>0.48199999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -4474,10 +4676,12 @@
         <v>3</v>
       </c>
       <c r="M39" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.02</v>
       </c>
       <c r="N39" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.02</v>
       </c>
       <c r="O39" t="str" cm="1">
         <f t="array" ref="O39">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K39,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K39,5), ",",".")</f>
@@ -4491,8 +4695,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K39,4), INDEX(Nodes!$A$3:$E$64,Arcs!L39,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K39,5), INDEX(Nodes!$A$3:$E$64,Arcs!L39,5)), ",", ".")</f>
         <v>7.22974632790087 65.3941076995608</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S39">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -4534,10 +4741,12 @@
         <v>37</v>
       </c>
       <c r="M40" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.05</v>
       </c>
       <c r="N40" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.05</v>
       </c>
       <c r="O40" t="str" cm="1">
         <f t="array" ref="O40">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K40,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K40,5), ",",".")</f>
@@ -4551,8 +4760,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K40,4), INDEX(Nodes!$A$3:$E$64,Arcs!L40,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K40,5), INDEX(Nodes!$A$3:$E$64,Arcs!L40,5)), ",", ".")</f>
         <v>4.83721350169052 60.5477617431823</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S40">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -4594,10 +4806,12 @@
         <v>48</v>
       </c>
       <c r="M41" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>9.4E-2</v>
       </c>
       <c r="N41" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>9.4E-2</v>
       </c>
       <c r="O41" t="str" cm="1">
         <f t="array" ref="O41">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K41,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K41,5), ",",".")</f>
@@ -4611,8 +4825,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K41,4), INDEX(Nodes!$A$3:$E$64,Arcs!L41,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K41,5), INDEX(Nodes!$A$3:$E$64,Arcs!L41,5)), ",", ".")</f>
         <v>1.82264345536872 59.1586920721751</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S41">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -4654,10 +4871,12 @@
         <v>16</v>
       </c>
       <c r="M42" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>3.9E-2</v>
       </c>
       <c r="N42" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>3.9E-2</v>
       </c>
       <c r="O42" t="str" cm="1">
         <f t="array" ref="O42">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K42,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K42,5), ",",".")</f>
@@ -4671,8 +4890,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K42,4), INDEX(Nodes!$A$3:$E$64,Arcs!L42,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K42,5), INDEX(Nodes!$A$3:$E$64,Arcs!L42,5)), ",", ".")</f>
         <v>2.19479968579955 58.2746767014261</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S42">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -4708,10 +4930,12 @@
         <v>9</v>
       </c>
       <c r="M43" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.1</v>
       </c>
       <c r="N43" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.1</v>
       </c>
       <c r="O43" t="str" cm="1">
         <f t="array" ref="O43">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K43,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K43,5), ",",".")</f>
@@ -4725,8 +4949,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K43,4), INDEX(Nodes!$A$3:$E$64,Arcs!L43,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K43,5), INDEX(Nodes!$A$3:$E$64,Arcs!L43,5)), ",", ".")</f>
         <v>7.45555 55.7275</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S43">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -4762,10 +4989,12 @@
         <v>11</v>
       </c>
       <c r="M44" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.05</v>
       </c>
       <c r="N44" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.05</v>
       </c>
       <c r="O44" t="str" cm="1">
         <f t="array" ref="O44">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K44,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K44,5), ",",".")</f>
@@ -4779,8 +5008,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K44,4), INDEX(Nodes!$A$3:$E$64,Arcs!L44,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K44,5), INDEX(Nodes!$A$3:$E$64,Arcs!L44,5)), ",", ".")</f>
         <v>10.05295 55.452</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S44">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -4816,10 +5048,12 @@
         <v>47</v>
       </c>
       <c r="M45" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.15</v>
       </c>
       <c r="N45" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="O45" t="str" cm="1">
         <f t="array" ref="O45">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K45,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K45,5), ",",".")</f>
@@ -4833,8 +5067,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K45,4), INDEX(Nodes!$A$3:$E$64,Arcs!L45,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K45,5), INDEX(Nodes!$A$3:$E$64,Arcs!L45,5)), ",", ".")</f>
         <v>13.23505 54.5945</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S45">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -4869,10 +5106,12 @@
         <v>55</v>
       </c>
       <c r="M46" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.2</v>
       </c>
       <c r="N46" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.2</v>
       </c>
       <c r="O46" t="str" cm="1">
         <f t="array" ref="O46">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K46,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K46,5), ",",".")</f>
@@ -4886,8 +5125,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K46,4), INDEX(Nodes!$A$3:$E$64,Arcs!L46,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K46,5), INDEX(Nodes!$A$3:$E$64,Arcs!L46,5)), ",", ".")</f>
         <v>0.349372 56.1913345</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S46">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -4911,7 +5153,7 @@
         <v>33</v>
       </c>
       <c r="J47" s="1" t="str">
-        <f t="shared" ref="J47:J55" si="2">IF(I47=100,"Capacity unknown","")</f>
+        <f t="shared" ref="J47:J55" si="4">IF(I47=100,"Capacity unknown","")</f>
         <v/>
       </c>
       <c r="K47" s="1">
@@ -4923,10 +5165,12 @@
         <v>52</v>
       </c>
       <c r="M47" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0.4</v>
       </c>
       <c r="N47" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0.4</v>
       </c>
       <c r="O47" t="str" cm="1">
         <f t="array" ref="O47">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K47,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K47,5), ",",".")</f>
@@ -4940,8 +5184,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K47,4), INDEX(Nodes!$A$3:$E$64,Arcs!L47,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K47,5), INDEX(Nodes!$A$3:$E$64,Arcs!L47,5)), ",", ".")</f>
         <v>-0.060319 59.307224</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S47">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -4962,7 +5209,7 @@
         <v>1000</v>
       </c>
       <c r="J48" s="30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K48" s="1">
@@ -4974,10 +5221,12 @@
         <v>10</v>
       </c>
       <c r="M48" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N48" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O48" t="str" cm="1">
         <f t="array" ref="O48">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K48,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K48,5), ",",".")</f>
@@ -4991,8 +5240,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K48,4), INDEX(Nodes!$A$3:$E$64,Arcs!L48,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K48,5), INDEX(Nodes!$A$3:$E$64,Arcs!L48,5)), ",", ".")</f>
         <v>8.85905 55.681</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -5013,7 +5265,7 @@
         <v>1000</v>
       </c>
       <c r="J49" s="30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K49" s="1">
@@ -5025,10 +5277,12 @@
         <v>12</v>
       </c>
       <c r="M49" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N49" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O49" t="str" cm="1">
         <f t="array" ref="O49">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K49,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K49,5), ",",".")</f>
@@ -5042,8 +5296,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K49,4), INDEX(Nodes!$A$3:$E$64,Arcs!L49,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K49,5), INDEX(Nodes!$A$3:$E$64,Arcs!L49,5)), ",", ".")</f>
         <v>11.00265 55.338</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -5064,7 +5321,7 @@
         <v>1000</v>
       </c>
       <c r="J50" s="30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K50" s="1">
@@ -5076,10 +5333,12 @@
         <v>15</v>
       </c>
       <c r="M50" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N50" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O50" t="str" cm="1">
         <f t="array" ref="O50">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K50,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K50,5), ",",".")</f>
@@ -5093,8 +5352,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K50,4), INDEX(Nodes!$A$3:$E$64,Arcs!L50,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K50,5), INDEX(Nodes!$A$3:$E$64,Arcs!L50,5)), ",", ".")</f>
         <v>2.46906857032826 58.1862791232136</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -5115,7 +5377,7 @@
         <v>1000</v>
       </c>
       <c r="J51" s="30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K51" s="1">
@@ -5127,10 +5389,12 @@
         <v>51</v>
       </c>
       <c r="M51" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N51" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O51" t="str" cm="1">
         <f t="array" ref="O51">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K51,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K51,5), ",",".")</f>
@@ -5144,8 +5408,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K51,4), INDEX(Nodes!$A$3:$E$64,Arcs!L51,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K51,5), INDEX(Nodes!$A$3:$E$64,Arcs!L51,5)), ",", ".")</f>
         <v>1.90731616528787 58.3677389907777</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -5166,7 +5433,7 @@
         <v>1000</v>
       </c>
       <c r="J52" s="30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K52" s="1">
@@ -5178,10 +5445,12 @@
         <v>43</v>
       </c>
       <c r="M52" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N52" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O52" t="str" cm="1">
         <f t="array" ref="O52">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K52,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K52,5), ",",".")</f>
@@ -5195,8 +5464,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K52,4), INDEX(Nodes!$A$3:$E$64,Arcs!L52,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K52,5), INDEX(Nodes!$A$3:$E$64,Arcs!L52,5)), ",", ".")</f>
         <v>3.28025150000001 56.5201845</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -5226,7 +5498,7 @@
         <v>1000</v>
       </c>
       <c r="J53" s="30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K53" s="1">
@@ -5238,10 +5510,12 @@
         <v>13</v>
       </c>
       <c r="M53" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N53" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O53" t="str" cm="1">
         <f t="array" ref="O53">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K53,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K53,5), ",",".")</f>
@@ -5255,8 +5529,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K53,4), INDEX(Nodes!$A$3:$E$64,Arcs!L53,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K53,5), INDEX(Nodes!$A$3:$E$64,Arcs!L53,5)), ",", ".")</f>
         <v>7.11614205264601 64.2919112956052</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -5286,7 +5563,7 @@
         <v>1000</v>
       </c>
       <c r="J54" s="30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K54" s="1">
@@ -5298,10 +5575,12 @@
         <v>40</v>
       </c>
       <c r="M54" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N54" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O54" t="str" cm="1">
         <f t="array" ref="O54">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K54,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K54,5), ",",".")</f>
@@ -5315,8 +5594,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K54,4), INDEX(Nodes!$A$3:$E$64,Arcs!L54,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K54,5), INDEX(Nodes!$A$3:$E$64,Arcs!L54,5)), ",", ".")</f>
         <v>1.70260105700003 61.0282477165</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -5346,7 +5628,7 @@
         <v>1000</v>
       </c>
       <c r="J55" s="30" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="K55" s="1">
@@ -5358,10 +5640,12 @@
         <v>2</v>
       </c>
       <c r="M55" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N55" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O55" t="str" cm="1">
         <f t="array" ref="O55">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K55,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K55,5), ",",".")</f>
@@ -5375,8 +5659,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K55,4), INDEX(Nodes!$A$3:$E$64,Arcs!L55,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K55,5), INDEX(Nodes!$A$3:$E$64,Arcs!L55,5)), ",", ".")</f>
         <v>5.74610048159499 63.6986000692747</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -5397,7 +5684,7 @@
         <v>1000</v>
       </c>
       <c r="J56" s="30" t="str">
-        <f t="shared" ref="J56:J60" si="3">IF(I56=100,"Capacity unknown","")</f>
+        <f t="shared" ref="J56:J60" si="5">IF(I56=100,"Capacity unknown","")</f>
         <v/>
       </c>
       <c r="K56" s="1">
@@ -5409,10 +5696,12 @@
         <v>46</v>
       </c>
       <c r="M56" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N56" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O56" t="str" cm="1">
         <f t="array" ref="O56">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K56,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K56,5), ",",".")</f>
@@ -5426,8 +5715,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K56,4), INDEX(Nodes!$A$3:$E$64,Arcs!L56,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K56,5), INDEX(Nodes!$A$3:$E$64,Arcs!L56,5)), ",", ".")</f>
         <v>2.93093584095346 60.5151147257528</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -5448,7 +5740,7 @@
         <v>1000</v>
       </c>
       <c r="J57" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K57" s="1">
@@ -5460,10 +5752,12 @@
         <v>2</v>
       </c>
       <c r="M57" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N57" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O57" t="str" cm="1">
         <f t="array" ref="O57">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K57,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K57,5), ",",".")</f>
@@ -5477,8 +5771,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K57,4), INDEX(Nodes!$A$3:$E$64,Arcs!L57,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K57,5), INDEX(Nodes!$A$3:$E$64,Arcs!L57,5)), ",", ".")</f>
         <v>6.23978361624093 63.3266481148799</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -5499,7 +5796,7 @@
         <v>1000</v>
       </c>
       <c r="J58" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K58" s="1">
@@ -5511,10 +5808,12 @@
         <v>34</v>
       </c>
       <c r="M58" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N58" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O58" t="str" cm="1">
         <f t="array" ref="O58">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K58,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K58,5), ",",".")</f>
@@ -5528,8 +5827,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K58,4), INDEX(Nodes!$A$3:$E$64,Arcs!L58,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K58,5), INDEX(Nodes!$A$3:$E$64,Arcs!L58,5)), ",", ".")</f>
         <v>3.65416291586873 59.0831068376751</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -5550,7 +5852,7 @@
         <v>1000</v>
       </c>
       <c r="J59" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K59" s="1">
@@ -5562,10 +5864,12 @@
         <v>36</v>
       </c>
       <c r="M59" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N59" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O59" t="str" cm="1">
         <f t="array" ref="O59">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K59,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K59,5), ",",".")</f>
@@ -5579,8 +5883,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K59,4), INDEX(Nodes!$A$3:$E$64,Arcs!L59,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K59,5), INDEX(Nodes!$A$3:$E$64,Arcs!L59,5)), ",", ".")</f>
         <v>4.03534642322643 59.0570233500857</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -5601,7 +5908,7 @@
         <v>1000</v>
       </c>
       <c r="J60" s="30" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="K60" s="1">
@@ -5613,10 +5920,12 @@
         <v>2</v>
       </c>
       <c r="M60" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N60" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O60" t="str" cm="1">
         <f t="array" ref="O60">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K60,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K60,5), ",",".")</f>
@@ -5630,8 +5939,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K60,4), INDEX(Nodes!$A$3:$E$64,Arcs!L60,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K60,5), INDEX(Nodes!$A$3:$E$64,Arcs!L60,5)), ",", ".")</f>
         <v>5.74500106359499 63.6936223192747</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -5652,7 +5964,7 @@
         <v>1000</v>
       </c>
       <c r="J61" s="30" t="str">
-        <f t="shared" ref="J61" si="4">IF(I61=100,"Capacity unknown","")</f>
+        <f t="shared" ref="J61" si="6">IF(I61=100,"Capacity unknown","")</f>
         <v/>
       </c>
       <c r="K61" s="1">
@@ -5664,10 +5976,12 @@
         <v>33</v>
       </c>
       <c r="M61" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N61" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O61" t="str" cm="1">
         <f t="array" ref="O61">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K61,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K61,5), ",",".")</f>
@@ -5681,8 +5995,11 @@
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K61,4), INDEX(Nodes!$A$3:$E$64,Arcs!L61,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K61,5), INDEX(Nodes!$A$3:$E$64,Arcs!L61,5)), ",", ".")</f>
         <v>2.12637048424656 59.7330186621066</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -5711,10 +6028,12 @@
         <v>24</v>
       </c>
       <c r="M62" s="2">
-        <v>1E-3</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="N62" s="3">
-        <v>1E-3</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O62" t="str" cm="1">
         <f t="array" ref="O62">SUBSTITUTE(INDEX(Nodes!$A$3:$E$64,Arcs!K62,4) &amp; " " &amp; INDEX(Nodes!$A$3:$E$64,Arcs!K62,5), ",",".")</f>
@@ -5727,6 +6046,9 @@
       <c r="Q62" t="str">
         <f>SUBSTITUTE(AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K62,4), INDEX(Nodes!$A$3:$E$64,Arcs!L62,4)) &amp; " " &amp; AVERAGE(INDEX(Nodes!$A$3:$E$64,Arcs!K62,5), INDEX(Nodes!$A$3:$E$64,Arcs!L62,5)), ",", ".")</f>
         <v>2.80258945333371 61.1761061046437</v>
+      </c>
+      <c r="S62">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5929,7 +6251,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6298,11 +6620,11 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:I10" si="0">SUM(C2:C9)</f>
+        <f>SUM(C2:C9)</f>
         <v>1</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f>SUM(D2:D9)</f>
         <v>1</v>
       </c>
       <c r="E10">
@@ -6314,15 +6636,15 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f>SUM(G2:G9)</f>
         <v>1</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f>SUM(H2:H9)</f>
         <v>1</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
+        <f>SUM(I2:I9)</f>
         <v>1</v>
       </c>
       <c r="L10" cm="1">
@@ -7636,7 +7958,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="A16:H16"/>
+      <selection activeCell="K16" sqref="K16:R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8224,8 +8546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3F5746-A1B1-6F4F-9762-CACD4A91B5F2}">
   <dimension ref="A1:AI64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="L1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8447,7 +8769,7 @@
         <v>10</v>
       </c>
       <c r="N3" s="2">
-        <f>IF(C3="Market",100,0)</f>
+        <f>IF(C3="Market",3000,0)</f>
         <v>0</v>
       </c>
       <c r="O3" s="2">
@@ -8561,7 +8883,7 @@
         <v>10</v>
       </c>
       <c r="N4" s="2">
-        <f t="shared" ref="N4:N61" si="1">IF(C4="Market",100,0)</f>
+        <f t="shared" ref="N4:N61" si="1">IF(C4="Market",3000,0)</f>
         <v>0</v>
       </c>
       <c r="O4" s="2">
@@ -10281,7 +10603,7 @@
       </c>
       <c r="N19" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="O19" s="2">
         <f t="shared" si="2"/>
@@ -10397,7 +10719,7 @@
       </c>
       <c r="N20" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="O20" s="2">
         <f t="shared" si="2"/>
@@ -10743,7 +11065,7 @@
       </c>
       <c r="N23" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="O23" s="2">
         <f t="shared" si="2"/>
@@ -10859,7 +11181,7 @@
       </c>
       <c r="N24" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="O24" s="2">
         <f t="shared" si="2"/>
@@ -13729,7 +14051,7 @@
       </c>
       <c r="N49" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="O49" s="2">
         <f t="shared" si="2"/>
@@ -14305,7 +14627,7 @@
       </c>
       <c r="N54" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="O54" s="2">
         <f t="shared" si="2"/>
@@ -14649,7 +14971,7 @@
       </c>
       <c r="N57" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="O57" s="2">
         <f t="shared" si="2"/>
@@ -14995,7 +15317,7 @@
       </c>
       <c r="N60" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>3000</v>
       </c>
       <c r="O60" s="2">
         <f t="shared" si="2"/>
@@ -15216,7 +15538,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16199,8 +16521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19292E87-5CF7-794D-A1AA-7C1926221C7B}">
   <dimension ref="A1:BM58"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="BE38" sqref="BE38"/>
+    <sheetView zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17649,11 +17971,11 @@
       </c>
       <c r="B9" s="2">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="11"/>
@@ -17689,11 +18011,11 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="2">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="S9" s="2">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="T9" s="2">
         <f t="shared" si="8"/>
@@ -17729,11 +18051,11 @@
       <c r="AG9" s="3"/>
       <c r="AH9" s="2">
         <f t="shared" si="13"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AI9" s="2">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AJ9" s="2">
         <f t="shared" si="9"/>
@@ -17769,11 +18091,11 @@
       <c r="AW9" s="3"/>
       <c r="AX9" s="2">
         <f t="shared" si="16"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AY9" s="2">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AZ9" s="2">
         <f t="shared" si="10"/>
@@ -18144,11 +18466,11 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="11"/>
@@ -18184,11 +18506,11 @@
       <c r="Q12" s="3"/>
       <c r="R12" s="2">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="S12" s="2">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="T12" s="2">
         <f t="shared" si="8"/>
@@ -18224,11 +18546,11 @@
       <c r="AG12" s="3"/>
       <c r="AH12" s="2">
         <f t="shared" si="13"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AI12" s="2">
         <f t="shared" si="9"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AJ12" s="2">
         <f t="shared" si="9"/>
@@ -18264,11 +18586,11 @@
       <c r="AW12" s="3"/>
       <c r="AX12" s="2">
         <f t="shared" si="16"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AY12" s="2">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AZ12" s="2">
         <f t="shared" si="10"/>
@@ -19821,10 +20143,10 @@
         <v>4</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -19845,10 +20167,10 @@
         <v>0</v>
       </c>
       <c r="R35">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="S35">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="T35">
         <v>0</v>
@@ -19869,10 +20191,10 @@
         <v>0</v>
       </c>
       <c r="AH35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ35">
         <v>0</v>
@@ -19893,10 +20215,10 @@
         <v>0</v>
       </c>
       <c r="AX35">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AY35">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AZ35">
         <v>0</v>
@@ -20124,10 +20446,10 @@
         <v>7</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -20148,10 +20470,10 @@
         <v>0</v>
       </c>
       <c r="R38">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="S38">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="T38">
         <v>0</v>
@@ -20172,10 +20494,10 @@
         <v>0</v>
       </c>
       <c r="AH38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI38">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ38">
         <v>0</v>
@@ -20196,10 +20518,10 @@
         <v>0</v>
       </c>
       <c r="AX38">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AY38">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AZ38">
         <v>0</v>
@@ -20542,6 +20864,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="R3:Y3"/>
+    <mergeCell ref="Z3:AG3"/>
     <mergeCell ref="AH1:AW1"/>
     <mergeCell ref="AH2:AW2"/>
     <mergeCell ref="AH3:AO3"/>
@@ -20550,14 +20880,6 @@
     <mergeCell ref="AX2:BM2"/>
     <mergeCell ref="AX3:BE3"/>
     <mergeCell ref="BF3:BM3"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="J3:Q3"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="R3:Y3"/>
-    <mergeCell ref="Z3:AG3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20567,8 +20889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7506CF-850A-ED42-956F-025E5A994524}">
   <dimension ref="A1:IW33"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="BQ6" sqref="BQ6"/>
+    <sheetView topLeftCell="IC3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="IH11" sqref="IH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21200,294 +21522,294 @@
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="61">
+      <c r="B3" s="64">
         <v>9</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62"/>
-      <c r="N3" s="62"/>
-      <c r="O3" s="62"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="61">
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="64">
         <v>9</v>
       </c>
-      <c r="S3" s="62"/>
-      <c r="T3" s="62"/>
-      <c r="U3" s="62"/>
-      <c r="V3" s="62"/>
-      <c r="W3" s="62"/>
-      <c r="X3" s="62"/>
-      <c r="Y3" s="62"/>
-      <c r="Z3" s="62"/>
-      <c r="AA3" s="62"/>
-      <c r="AB3" s="62"/>
-      <c r="AC3" s="62"/>
-      <c r="AD3" s="62"/>
-      <c r="AE3" s="62"/>
-      <c r="AF3" s="62"/>
-      <c r="AG3" s="63"/>
-      <c r="AH3" s="61">
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
+      <c r="Y3" s="65"/>
+      <c r="Z3" s="65"/>
+      <c r="AA3" s="65"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
+      <c r="AE3" s="65"/>
+      <c r="AF3" s="65"/>
+      <c r="AG3" s="66"/>
+      <c r="AH3" s="64">
         <v>9</v>
       </c>
-      <c r="AI3" s="62"/>
-      <c r="AJ3" s="62"/>
-      <c r="AK3" s="62"/>
-      <c r="AL3" s="62"/>
-      <c r="AM3" s="62"/>
-      <c r="AN3" s="62"/>
-      <c r="AO3" s="62"/>
-      <c r="AP3" s="62"/>
-      <c r="AQ3" s="62"/>
-      <c r="AR3" s="62"/>
-      <c r="AS3" s="62"/>
-      <c r="AT3" s="62"/>
-      <c r="AU3" s="62"/>
-      <c r="AV3" s="62"/>
-      <c r="AW3" s="63"/>
-      <c r="AX3" s="61">
+      <c r="AI3" s="65"/>
+      <c r="AJ3" s="65"/>
+      <c r="AK3" s="65"/>
+      <c r="AL3" s="65"/>
+      <c r="AM3" s="65"/>
+      <c r="AN3" s="65"/>
+      <c r="AO3" s="65"/>
+      <c r="AP3" s="65"/>
+      <c r="AQ3" s="65"/>
+      <c r="AR3" s="65"/>
+      <c r="AS3" s="65"/>
+      <c r="AT3" s="65"/>
+      <c r="AU3" s="65"/>
+      <c r="AV3" s="65"/>
+      <c r="AW3" s="66"/>
+      <c r="AX3" s="64">
         <v>9</v>
       </c>
-      <c r="AY3" s="62"/>
-      <c r="AZ3" s="62"/>
-      <c r="BA3" s="62"/>
-      <c r="BB3" s="62"/>
-      <c r="BC3" s="62"/>
-      <c r="BD3" s="62"/>
-      <c r="BE3" s="62"/>
-      <c r="BF3" s="62"/>
-      <c r="BG3" s="62"/>
-      <c r="BH3" s="62"/>
-      <c r="BI3" s="62"/>
-      <c r="BJ3" s="62"/>
-      <c r="BK3" s="62"/>
-      <c r="BL3" s="62"/>
-      <c r="BM3" s="63"/>
-      <c r="BN3" s="61">
+      <c r="AY3" s="65"/>
+      <c r="AZ3" s="65"/>
+      <c r="BA3" s="65"/>
+      <c r="BB3" s="65"/>
+      <c r="BC3" s="65"/>
+      <c r="BD3" s="65"/>
+      <c r="BE3" s="65"/>
+      <c r="BF3" s="65"/>
+      <c r="BG3" s="65"/>
+      <c r="BH3" s="65"/>
+      <c r="BI3" s="65"/>
+      <c r="BJ3" s="65"/>
+      <c r="BK3" s="65"/>
+      <c r="BL3" s="65"/>
+      <c r="BM3" s="66"/>
+      <c r="BN3" s="64">
         <v>17</v>
       </c>
-      <c r="BO3" s="62"/>
-      <c r="BP3" s="62"/>
-      <c r="BQ3" s="62"/>
-      <c r="BR3" s="62"/>
-      <c r="BS3" s="62"/>
-      <c r="BT3" s="62"/>
-      <c r="BU3" s="62"/>
-      <c r="BV3" s="62"/>
-      <c r="BW3" s="62"/>
-      <c r="BX3" s="62"/>
-      <c r="BY3" s="62"/>
-      <c r="BZ3" s="62"/>
-      <c r="CA3" s="62"/>
-      <c r="CB3" s="62"/>
-      <c r="CC3" s="63"/>
-      <c r="CD3" s="61">
+      <c r="BO3" s="65"/>
+      <c r="BP3" s="65"/>
+      <c r="BQ3" s="65"/>
+      <c r="BR3" s="65"/>
+      <c r="BS3" s="65"/>
+      <c r="BT3" s="65"/>
+      <c r="BU3" s="65"/>
+      <c r="BV3" s="65"/>
+      <c r="BW3" s="65"/>
+      <c r="BX3" s="65"/>
+      <c r="BY3" s="65"/>
+      <c r="BZ3" s="65"/>
+      <c r="CA3" s="65"/>
+      <c r="CB3" s="65"/>
+      <c r="CC3" s="66"/>
+      <c r="CD3" s="64">
         <v>17</v>
       </c>
-      <c r="CE3" s="62"/>
-      <c r="CF3" s="62"/>
-      <c r="CG3" s="62"/>
-      <c r="CH3" s="62"/>
-      <c r="CI3" s="62"/>
-      <c r="CJ3" s="62"/>
-      <c r="CK3" s="62"/>
-      <c r="CL3" s="62"/>
-      <c r="CM3" s="62"/>
-      <c r="CN3" s="62"/>
-      <c r="CO3" s="62"/>
-      <c r="CP3" s="62"/>
-      <c r="CQ3" s="62"/>
-      <c r="CR3" s="62"/>
-      <c r="CS3" s="63"/>
-      <c r="CT3" s="61">
+      <c r="CE3" s="65"/>
+      <c r="CF3" s="65"/>
+      <c r="CG3" s="65"/>
+      <c r="CH3" s="65"/>
+      <c r="CI3" s="65"/>
+      <c r="CJ3" s="65"/>
+      <c r="CK3" s="65"/>
+      <c r="CL3" s="65"/>
+      <c r="CM3" s="65"/>
+      <c r="CN3" s="65"/>
+      <c r="CO3" s="65"/>
+      <c r="CP3" s="65"/>
+      <c r="CQ3" s="65"/>
+      <c r="CR3" s="65"/>
+      <c r="CS3" s="66"/>
+      <c r="CT3" s="64">
         <v>17</v>
       </c>
-      <c r="CU3" s="62"/>
-      <c r="CV3" s="62"/>
-      <c r="CW3" s="62"/>
-      <c r="CX3" s="62"/>
-      <c r="CY3" s="62"/>
-      <c r="CZ3" s="62"/>
-      <c r="DA3" s="62"/>
-      <c r="DB3" s="62"/>
-      <c r="DC3" s="62"/>
-      <c r="DD3" s="62"/>
-      <c r="DE3" s="62"/>
-      <c r="DF3" s="62"/>
-      <c r="DG3" s="62"/>
-      <c r="DH3" s="62"/>
-      <c r="DI3" s="63"/>
-      <c r="DJ3" s="61">
+      <c r="CU3" s="65"/>
+      <c r="CV3" s="65"/>
+      <c r="CW3" s="65"/>
+      <c r="CX3" s="65"/>
+      <c r="CY3" s="65"/>
+      <c r="CZ3" s="65"/>
+      <c r="DA3" s="65"/>
+      <c r="DB3" s="65"/>
+      <c r="DC3" s="65"/>
+      <c r="DD3" s="65"/>
+      <c r="DE3" s="65"/>
+      <c r="DF3" s="65"/>
+      <c r="DG3" s="65"/>
+      <c r="DH3" s="65"/>
+      <c r="DI3" s="66"/>
+      <c r="DJ3" s="64">
         <v>17</v>
       </c>
-      <c r="DK3" s="62"/>
-      <c r="DL3" s="62"/>
-      <c r="DM3" s="62"/>
-      <c r="DN3" s="62"/>
-      <c r="DO3" s="62"/>
-      <c r="DP3" s="62"/>
-      <c r="DQ3" s="62"/>
-      <c r="DR3" s="62"/>
-      <c r="DS3" s="62"/>
-      <c r="DT3" s="62"/>
-      <c r="DU3" s="62"/>
-      <c r="DV3" s="62"/>
-      <c r="DW3" s="62"/>
-      <c r="DX3" s="62"/>
-      <c r="DY3" s="63"/>
-      <c r="DZ3" s="64">
+      <c r="DK3" s="65"/>
+      <c r="DL3" s="65"/>
+      <c r="DM3" s="65"/>
+      <c r="DN3" s="65"/>
+      <c r="DO3" s="65"/>
+      <c r="DP3" s="65"/>
+      <c r="DQ3" s="65"/>
+      <c r="DR3" s="65"/>
+      <c r="DS3" s="65"/>
+      <c r="DT3" s="65"/>
+      <c r="DU3" s="65"/>
+      <c r="DV3" s="65"/>
+      <c r="DW3" s="65"/>
+      <c r="DX3" s="65"/>
+      <c r="DY3" s="66"/>
+      <c r="DZ3" s="67">
         <v>25</v>
       </c>
-      <c r="EA3" s="65"/>
-      <c r="EB3" s="65"/>
-      <c r="EC3" s="65"/>
-      <c r="ED3" s="65"/>
-      <c r="EE3" s="65"/>
-      <c r="EF3" s="65"/>
-      <c r="EG3" s="65"/>
-      <c r="EH3" s="65"/>
-      <c r="EI3" s="65"/>
-      <c r="EJ3" s="65"/>
-      <c r="EK3" s="65"/>
-      <c r="EL3" s="65"/>
-      <c r="EM3" s="65"/>
-      <c r="EN3" s="65"/>
-      <c r="EO3" s="66"/>
-      <c r="EP3" s="67">
+      <c r="EA3" s="62"/>
+      <c r="EB3" s="62"/>
+      <c r="EC3" s="62"/>
+      <c r="ED3" s="62"/>
+      <c r="EE3" s="62"/>
+      <c r="EF3" s="62"/>
+      <c r="EG3" s="62"/>
+      <c r="EH3" s="62"/>
+      <c r="EI3" s="62"/>
+      <c r="EJ3" s="62"/>
+      <c r="EK3" s="62"/>
+      <c r="EL3" s="62"/>
+      <c r="EM3" s="62"/>
+      <c r="EN3" s="62"/>
+      <c r="EO3" s="63"/>
+      <c r="EP3" s="61">
         <v>25</v>
       </c>
-      <c r="EQ3" s="65"/>
-      <c r="ER3" s="65"/>
-      <c r="ES3" s="65"/>
-      <c r="ET3" s="65"/>
-      <c r="EU3" s="65"/>
-      <c r="EV3" s="65"/>
-      <c r="EW3" s="65"/>
-      <c r="EX3" s="65"/>
-      <c r="EY3" s="65"/>
-      <c r="EZ3" s="65"/>
-      <c r="FA3" s="65"/>
-      <c r="FB3" s="65"/>
-      <c r="FC3" s="65"/>
-      <c r="FD3" s="65"/>
-      <c r="FE3" s="66"/>
-      <c r="FF3" s="67">
+      <c r="EQ3" s="62"/>
+      <c r="ER3" s="62"/>
+      <c r="ES3" s="62"/>
+      <c r="ET3" s="62"/>
+      <c r="EU3" s="62"/>
+      <c r="EV3" s="62"/>
+      <c r="EW3" s="62"/>
+      <c r="EX3" s="62"/>
+      <c r="EY3" s="62"/>
+      <c r="EZ3" s="62"/>
+      <c r="FA3" s="62"/>
+      <c r="FB3" s="62"/>
+      <c r="FC3" s="62"/>
+      <c r="FD3" s="62"/>
+      <c r="FE3" s="63"/>
+      <c r="FF3" s="61">
         <v>25</v>
       </c>
-      <c r="FG3" s="65"/>
-      <c r="FH3" s="65"/>
-      <c r="FI3" s="65"/>
-      <c r="FJ3" s="65"/>
-      <c r="FK3" s="65"/>
-      <c r="FL3" s="65"/>
-      <c r="FM3" s="65"/>
-      <c r="FN3" s="65"/>
-      <c r="FO3" s="65"/>
-      <c r="FP3" s="65"/>
-      <c r="FQ3" s="65"/>
-      <c r="FR3" s="65"/>
-      <c r="FS3" s="65"/>
-      <c r="FT3" s="65"/>
-      <c r="FU3" s="66"/>
-      <c r="FV3" s="67">
+      <c r="FG3" s="62"/>
+      <c r="FH3" s="62"/>
+      <c r="FI3" s="62"/>
+      <c r="FJ3" s="62"/>
+      <c r="FK3" s="62"/>
+      <c r="FL3" s="62"/>
+      <c r="FM3" s="62"/>
+      <c r="FN3" s="62"/>
+      <c r="FO3" s="62"/>
+      <c r="FP3" s="62"/>
+      <c r="FQ3" s="62"/>
+      <c r="FR3" s="62"/>
+      <c r="FS3" s="62"/>
+      <c r="FT3" s="62"/>
+      <c r="FU3" s="63"/>
+      <c r="FV3" s="61">
         <v>25</v>
       </c>
-      <c r="FW3" s="65"/>
-      <c r="FX3" s="65"/>
-      <c r="FY3" s="65"/>
-      <c r="FZ3" s="65"/>
-      <c r="GA3" s="65"/>
-      <c r="GB3" s="65"/>
-      <c r="GC3" s="65"/>
-      <c r="GD3" s="65"/>
-      <c r="GE3" s="65"/>
-      <c r="GF3" s="65"/>
-      <c r="GG3" s="65"/>
-      <c r="GH3" s="65"/>
-      <c r="GI3" s="65"/>
-      <c r="GJ3" s="65"/>
-      <c r="GK3" s="66"/>
-      <c r="GL3" s="67">
+      <c r="FW3" s="62"/>
+      <c r="FX3" s="62"/>
+      <c r="FY3" s="62"/>
+      <c r="FZ3" s="62"/>
+      <c r="GA3" s="62"/>
+      <c r="GB3" s="62"/>
+      <c r="GC3" s="62"/>
+      <c r="GD3" s="62"/>
+      <c r="GE3" s="62"/>
+      <c r="GF3" s="62"/>
+      <c r="GG3" s="62"/>
+      <c r="GH3" s="62"/>
+      <c r="GI3" s="62"/>
+      <c r="GJ3" s="62"/>
+      <c r="GK3" s="63"/>
+      <c r="GL3" s="61">
         <v>33</v>
       </c>
-      <c r="GM3" s="65"/>
-      <c r="GN3" s="65"/>
-      <c r="GO3" s="65"/>
-      <c r="GP3" s="65"/>
-      <c r="GQ3" s="65"/>
-      <c r="GR3" s="65"/>
-      <c r="GS3" s="65"/>
-      <c r="GT3" s="65"/>
-      <c r="GU3" s="65"/>
-      <c r="GV3" s="65"/>
-      <c r="GW3" s="65"/>
-      <c r="GX3" s="65"/>
-      <c r="GY3" s="65"/>
-      <c r="GZ3" s="65"/>
-      <c r="HA3" s="66"/>
-      <c r="HB3" s="67">
+      <c r="GM3" s="62"/>
+      <c r="GN3" s="62"/>
+      <c r="GO3" s="62"/>
+      <c r="GP3" s="62"/>
+      <c r="GQ3" s="62"/>
+      <c r="GR3" s="62"/>
+      <c r="GS3" s="62"/>
+      <c r="GT3" s="62"/>
+      <c r="GU3" s="62"/>
+      <c r="GV3" s="62"/>
+      <c r="GW3" s="62"/>
+      <c r="GX3" s="62"/>
+      <c r="GY3" s="62"/>
+      <c r="GZ3" s="62"/>
+      <c r="HA3" s="63"/>
+      <c r="HB3" s="61">
         <v>33</v>
       </c>
-      <c r="HC3" s="65"/>
-      <c r="HD3" s="65"/>
-      <c r="HE3" s="65"/>
-      <c r="HF3" s="65"/>
-      <c r="HG3" s="65"/>
-      <c r="HH3" s="65"/>
-      <c r="HI3" s="65"/>
-      <c r="HJ3" s="65"/>
-      <c r="HK3" s="65"/>
-      <c r="HL3" s="65"/>
-      <c r="HM3" s="65"/>
-      <c r="HN3" s="65"/>
-      <c r="HO3" s="65"/>
-      <c r="HP3" s="65"/>
-      <c r="HQ3" s="66"/>
-      <c r="HR3" s="67">
+      <c r="HC3" s="62"/>
+      <c r="HD3" s="62"/>
+      <c r="HE3" s="62"/>
+      <c r="HF3" s="62"/>
+      <c r="HG3" s="62"/>
+      <c r="HH3" s="62"/>
+      <c r="HI3" s="62"/>
+      <c r="HJ3" s="62"/>
+      <c r="HK3" s="62"/>
+      <c r="HL3" s="62"/>
+      <c r="HM3" s="62"/>
+      <c r="HN3" s="62"/>
+      <c r="HO3" s="62"/>
+      <c r="HP3" s="62"/>
+      <c r="HQ3" s="63"/>
+      <c r="HR3" s="61">
         <v>33</v>
       </c>
-      <c r="HS3" s="65"/>
-      <c r="HT3" s="65"/>
-      <c r="HU3" s="65"/>
-      <c r="HV3" s="65"/>
-      <c r="HW3" s="65"/>
-      <c r="HX3" s="65"/>
-      <c r="HY3" s="65"/>
-      <c r="HZ3" s="65"/>
-      <c r="IA3" s="65"/>
-      <c r="IB3" s="65"/>
-      <c r="IC3" s="65"/>
-      <c r="ID3" s="65"/>
-      <c r="IE3" s="65"/>
-      <c r="IF3" s="65"/>
-      <c r="IG3" s="66"/>
-      <c r="IH3" s="67">
+      <c r="HS3" s="62"/>
+      <c r="HT3" s="62"/>
+      <c r="HU3" s="62"/>
+      <c r="HV3" s="62"/>
+      <c r="HW3" s="62"/>
+      <c r="HX3" s="62"/>
+      <c r="HY3" s="62"/>
+      <c r="HZ3" s="62"/>
+      <c r="IA3" s="62"/>
+      <c r="IB3" s="62"/>
+      <c r="IC3" s="62"/>
+      <c r="ID3" s="62"/>
+      <c r="IE3" s="62"/>
+      <c r="IF3" s="62"/>
+      <c r="IG3" s="63"/>
+      <c r="IH3" s="61">
         <v>33</v>
       </c>
-      <c r="II3" s="65"/>
-      <c r="IJ3" s="65"/>
-      <c r="IK3" s="65"/>
-      <c r="IL3" s="65"/>
-      <c r="IM3" s="65"/>
-      <c r="IN3" s="65"/>
-      <c r="IO3" s="65"/>
-      <c r="IP3" s="65"/>
-      <c r="IQ3" s="65"/>
-      <c r="IR3" s="65"/>
-      <c r="IS3" s="65"/>
-      <c r="IT3" s="65"/>
-      <c r="IU3" s="65"/>
-      <c r="IV3" s="65"/>
-      <c r="IW3" s="66"/>
+      <c r="II3" s="62"/>
+      <c r="IJ3" s="62"/>
+      <c r="IK3" s="62"/>
+      <c r="IL3" s="62"/>
+      <c r="IM3" s="62"/>
+      <c r="IN3" s="62"/>
+      <c r="IO3" s="62"/>
+      <c r="IP3" s="62"/>
+      <c r="IQ3" s="62"/>
+      <c r="IR3" s="62"/>
+      <c r="IS3" s="62"/>
+      <c r="IT3" s="62"/>
+      <c r="IU3" s="62"/>
+      <c r="IV3" s="62"/>
+      <c r="IW3" s="63"/>
     </row>
     <row r="4" spans="1:257" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
@@ -26963,11 +27285,11 @@
       </c>
       <c r="B10" s="2">
         <f>'Demand Stage 2'!B9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2">
         <f>'Demand Stage 2'!C9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2">
         <f>'Demand Stage 2'!D9</f>
@@ -27003,11 +27325,11 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="2">
         <f>'Demand Stage 2'!B9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="S10" s="2">
         <f>'Demand Stage 2'!C9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="T10" s="2">
         <f>'Demand Stage 2'!D9</f>
@@ -27043,11 +27365,11 @@
       <c r="AG10" s="3"/>
       <c r="AH10" s="2">
         <f>'Demand Stage 2'!B9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AI10" s="2">
         <f>'Demand Stage 2'!C9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AJ10" s="2">
         <f>'Demand Stage 2'!D9</f>
@@ -27083,11 +27405,11 @@
       <c r="AW10" s="3"/>
       <c r="AX10" s="2">
         <f>'Demand Stage 2'!B9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AY10" s="2">
         <f>'Demand Stage 2'!C9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AZ10" s="2">
         <f>'Demand Stage 2'!D9</f>
@@ -27123,11 +27445,11 @@
       <c r="BM10" s="3"/>
       <c r="BN10" s="2">
         <f>'Demand Stage 2'!R9</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BO10" s="2">
         <f>'Demand Stage 2'!S9</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BP10" s="2">
         <f>'Demand Stage 2'!T9</f>
@@ -27163,11 +27485,11 @@
       <c r="CC10" s="3"/>
       <c r="CD10" s="2">
         <f t="shared" si="38"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="CE10" s="2">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="CF10" s="2">
         <f t="shared" si="14"/>
@@ -27203,11 +27525,11 @@
       <c r="CS10" s="3"/>
       <c r="CT10" s="2">
         <f t="shared" si="74"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="CU10" s="2">
         <f t="shared" si="16"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="CV10" s="2">
         <f t="shared" si="16"/>
@@ -27243,11 +27565,11 @@
       <c r="DI10" s="3"/>
       <c r="DJ10" s="2">
         <f t="shared" si="40"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="DK10" s="2">
         <f t="shared" si="24"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="DL10" s="2">
         <f t="shared" si="24"/>
@@ -27283,11 +27605,11 @@
       <c r="DY10" s="3"/>
       <c r="DZ10" s="2">
         <f>'Demand Stage 2'!AH9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="EA10" s="2">
         <f>'Demand Stage 2'!AI9</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="EB10" s="2">
         <f>'Demand Stage 2'!AJ9</f>
@@ -27323,11 +27645,11 @@
       <c r="EO10" s="3"/>
       <c r="EP10" s="2">
         <f t="shared" si="49"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="EQ10" s="2">
         <f t="shared" si="26"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="ER10" s="2">
         <f t="shared" si="26"/>
@@ -27363,11 +27685,11 @@
       <c r="FE10" s="3"/>
       <c r="FF10" s="2">
         <f t="shared" si="51"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="FG10" s="2">
         <f t="shared" si="28"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="FH10" s="2">
         <f t="shared" si="28"/>
@@ -27403,11 +27725,11 @@
       <c r="FU10" s="3"/>
       <c r="FV10" s="2">
         <f t="shared" si="60"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="FW10" s="2">
         <f t="shared" si="30"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="FX10" s="2">
         <f t="shared" si="30"/>
@@ -27443,11 +27765,11 @@
       <c r="GK10" s="3"/>
       <c r="GL10" s="2">
         <f>'Demand Stage 2'!AX9</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="GM10" s="2">
         <f>'Demand Stage 2'!AY9</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="GN10" s="2">
         <f>'Demand Stage 2'!AZ9</f>
@@ -27483,11 +27805,11 @@
       <c r="HA10" s="3"/>
       <c r="HB10" s="2">
         <f t="shared" si="75"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="HC10" s="2">
         <f t="shared" si="32"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="HD10" s="2">
         <f t="shared" si="32"/>
@@ -27523,11 +27845,11 @@
       <c r="HQ10" s="3"/>
       <c r="HR10" s="2">
         <f t="shared" si="70"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="HS10" s="2">
         <f t="shared" si="34"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="HT10" s="2">
         <f t="shared" si="34"/>
@@ -27563,11 +27885,11 @@
       <c r="IG10" s="3"/>
       <c r="IH10" s="2">
         <f t="shared" si="72"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="II10" s="2">
         <f t="shared" si="36"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="IJ10" s="2">
         <f t="shared" si="36"/>
@@ -28898,11 +29220,11 @@
       </c>
       <c r="B13" s="2">
         <f>'Demand Stage 2'!B12</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C13" s="2">
         <f>'Demand Stage 2'!C12</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2">
         <f>'Demand Stage 2'!D12</f>
@@ -28938,11 +29260,11 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="2">
         <f>'Demand Stage 2'!B12</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="S13" s="2">
         <f>'Demand Stage 2'!C12</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="T13" s="2">
         <f>'Demand Stage 2'!D12</f>
@@ -28978,11 +29300,11 @@
       <c r="AG13" s="3"/>
       <c r="AH13" s="2">
         <f>'Demand Stage 2'!B12</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AI13" s="2">
         <f>'Demand Stage 2'!C12</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AJ13" s="2">
         <f>'Demand Stage 2'!D12</f>
@@ -29018,11 +29340,11 @@
       <c r="AW13" s="3"/>
       <c r="AX13" s="2">
         <f>'Demand Stage 2'!B12</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AY13" s="2">
         <f>'Demand Stage 2'!C12</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AZ13" s="2">
         <f>'Demand Stage 2'!D12</f>
@@ -29058,11 +29380,11 @@
       <c r="BM13" s="3"/>
       <c r="BN13" s="2">
         <f>'Demand Stage 2'!R12</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BO13" s="2">
         <f>'Demand Stage 2'!S12</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="BP13" s="2">
         <f>'Demand Stage 2'!T12</f>
@@ -29098,11 +29420,11 @@
       <c r="CC13" s="3"/>
       <c r="CD13" s="2">
         <f t="shared" si="38"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="CE13" s="2">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="CF13" s="2">
         <f t="shared" si="14"/>
@@ -29138,11 +29460,11 @@
       <c r="CS13" s="3"/>
       <c r="CT13" s="2">
         <f t="shared" si="74"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="CU13" s="2">
         <f t="shared" si="16"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="CV13" s="2">
         <f t="shared" si="16"/>
@@ -29178,11 +29500,11 @@
       <c r="DI13" s="3"/>
       <c r="DJ13" s="2">
         <f t="shared" si="40"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="DK13" s="2">
         <f t="shared" si="24"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="DL13" s="2">
         <f t="shared" si="24"/>
@@ -29218,11 +29540,11 @@
       <c r="DY13" s="3"/>
       <c r="DZ13" s="2">
         <f>'Demand Stage 2'!AH12</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="EA13" s="2">
         <f>'Demand Stage 2'!AI12</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="EB13" s="2">
         <f>'Demand Stage 2'!AJ12</f>
@@ -29258,11 +29580,11 @@
       <c r="EO13" s="3"/>
       <c r="EP13" s="2">
         <f t="shared" si="49"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="EQ13" s="2">
         <f t="shared" si="26"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="ER13" s="2">
         <f t="shared" si="26"/>
@@ -29298,11 +29620,11 @@
       <c r="FE13" s="3"/>
       <c r="FF13" s="2">
         <f t="shared" si="51"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="FG13" s="2">
         <f t="shared" si="28"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="FH13" s="2">
         <f t="shared" si="28"/>
@@ -29338,11 +29660,11 @@
       <c r="FU13" s="3"/>
       <c r="FV13" s="2">
         <f t="shared" si="60"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="FW13" s="2">
         <f t="shared" si="30"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="FX13" s="2">
         <f t="shared" si="30"/>
@@ -29378,11 +29700,11 @@
       <c r="GK13" s="3"/>
       <c r="GL13" s="2">
         <f>'Demand Stage 2'!AX12</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="GM13" s="2">
         <f>'Demand Stage 2'!AY12</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="GN13" s="2">
         <f>'Demand Stage 2'!AZ12</f>
@@ -29418,11 +29740,11 @@
       <c r="HA13" s="3"/>
       <c r="HB13" s="2">
         <f t="shared" si="75"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="HC13" s="2">
         <f t="shared" si="32"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="HD13" s="2">
         <f t="shared" si="32"/>
@@ -29458,11 +29780,11 @@
       <c r="HQ13" s="3"/>
       <c r="HR13" s="2">
         <f t="shared" si="70"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="HS13" s="2">
         <f t="shared" si="34"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="HT13" s="2">
         <f t="shared" si="34"/>
@@ -29498,11 +29820,11 @@
       <c r="IG13" s="3"/>
       <c r="IH13" s="2">
         <f t="shared" si="72"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="II13" s="2">
         <f t="shared" si="36"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="IJ13" s="2">
         <f t="shared" si="36"/>
@@ -33724,19 +34046,57 @@
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="HB2:HQ2"/>
-    <mergeCell ref="HR2:IG2"/>
-    <mergeCell ref="IH2:IW2"/>
-    <mergeCell ref="DZ2:EO2"/>
-    <mergeCell ref="EP2:FE2"/>
-    <mergeCell ref="FF2:FU2"/>
-    <mergeCell ref="FV2:GK2"/>
-    <mergeCell ref="GL2:HA2"/>
-    <mergeCell ref="AX2:BM2"/>
-    <mergeCell ref="BN2:CC2"/>
-    <mergeCell ref="CD2:CS2"/>
-    <mergeCell ref="CT2:DI2"/>
-    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="R1:AG1"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R2:AG2"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="J4:Q4"/>
+    <mergeCell ref="R4:Y4"/>
+    <mergeCell ref="Z4:AG4"/>
+    <mergeCell ref="B3:Q3"/>
+    <mergeCell ref="R3:AG3"/>
+    <mergeCell ref="AH4:AO4"/>
+    <mergeCell ref="AP4:AW4"/>
+    <mergeCell ref="AX4:BE4"/>
+    <mergeCell ref="BF4:BM4"/>
+    <mergeCell ref="BN4:BU4"/>
+    <mergeCell ref="BV4:CC4"/>
+    <mergeCell ref="CD4:CK4"/>
+    <mergeCell ref="CL4:CS4"/>
+    <mergeCell ref="CT4:DA4"/>
+    <mergeCell ref="DB4:DI4"/>
+    <mergeCell ref="DJ4:DQ4"/>
+    <mergeCell ref="DR4:DY4"/>
+    <mergeCell ref="DZ4:EG4"/>
+    <mergeCell ref="EH4:EO4"/>
+    <mergeCell ref="EP4:EW4"/>
+    <mergeCell ref="EX4:FE4"/>
+    <mergeCell ref="FF4:FM4"/>
+    <mergeCell ref="FN4:FU4"/>
+    <mergeCell ref="FV4:GC4"/>
+    <mergeCell ref="GD4:GK4"/>
+    <mergeCell ref="GL4:GS4"/>
+    <mergeCell ref="GT4:HA4"/>
+    <mergeCell ref="HB4:HI4"/>
+    <mergeCell ref="HJ4:HQ4"/>
+    <mergeCell ref="HR4:HY4"/>
+    <mergeCell ref="HZ4:IG4"/>
+    <mergeCell ref="IH4:IO4"/>
+    <mergeCell ref="IP4:IW4"/>
+    <mergeCell ref="AH3:AW3"/>
+    <mergeCell ref="AX3:BM3"/>
+    <mergeCell ref="BN3:CC3"/>
+    <mergeCell ref="CD3:CS3"/>
+    <mergeCell ref="CT3:DI3"/>
+    <mergeCell ref="DJ3:DY3"/>
+    <mergeCell ref="DZ3:EO3"/>
+    <mergeCell ref="EP3:FE3"/>
+    <mergeCell ref="FF3:FU3"/>
+    <mergeCell ref="FV3:GK3"/>
+    <mergeCell ref="GL3:HA3"/>
+    <mergeCell ref="HB3:HQ3"/>
+    <mergeCell ref="HR3:IG3"/>
     <mergeCell ref="IH3:IW3"/>
     <mergeCell ref="AH1:AW1"/>
     <mergeCell ref="AX1:BM1"/>
@@ -33753,57 +34113,19 @@
     <mergeCell ref="HR1:IG1"/>
     <mergeCell ref="IH1:IW1"/>
     <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="HZ4:IG4"/>
-    <mergeCell ref="IH4:IO4"/>
-    <mergeCell ref="IP4:IW4"/>
-    <mergeCell ref="AH3:AW3"/>
-    <mergeCell ref="AX3:BM3"/>
-    <mergeCell ref="BN3:CC3"/>
-    <mergeCell ref="CD3:CS3"/>
-    <mergeCell ref="CT3:DI3"/>
-    <mergeCell ref="DJ3:DY3"/>
-    <mergeCell ref="DZ3:EO3"/>
-    <mergeCell ref="EP3:FE3"/>
-    <mergeCell ref="FF3:FU3"/>
-    <mergeCell ref="FV3:GK3"/>
-    <mergeCell ref="GL3:HA3"/>
-    <mergeCell ref="HB3:HQ3"/>
-    <mergeCell ref="HR3:IG3"/>
-    <mergeCell ref="GL4:GS4"/>
-    <mergeCell ref="GT4:HA4"/>
-    <mergeCell ref="HB4:HI4"/>
-    <mergeCell ref="HJ4:HQ4"/>
-    <mergeCell ref="HR4:HY4"/>
-    <mergeCell ref="EX4:FE4"/>
-    <mergeCell ref="FF4:FM4"/>
-    <mergeCell ref="FN4:FU4"/>
-    <mergeCell ref="FV4:GC4"/>
-    <mergeCell ref="GD4:GK4"/>
-    <mergeCell ref="DJ4:DQ4"/>
-    <mergeCell ref="DR4:DY4"/>
-    <mergeCell ref="DZ4:EG4"/>
-    <mergeCell ref="EH4:EO4"/>
-    <mergeCell ref="EP4:EW4"/>
-    <mergeCell ref="BV4:CC4"/>
-    <mergeCell ref="CD4:CK4"/>
-    <mergeCell ref="CL4:CS4"/>
-    <mergeCell ref="CT4:DA4"/>
-    <mergeCell ref="DB4:DI4"/>
-    <mergeCell ref="AH4:AO4"/>
-    <mergeCell ref="AP4:AW4"/>
-    <mergeCell ref="AX4:BE4"/>
-    <mergeCell ref="BF4:BM4"/>
-    <mergeCell ref="BN4:BU4"/>
-    <mergeCell ref="B1:Q1"/>
-    <mergeCell ref="R1:AG1"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="R2:AG2"/>
-    <mergeCell ref="B4:I4"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="R4:Y4"/>
-    <mergeCell ref="Z4:AG4"/>
-    <mergeCell ref="B3:Q3"/>
-    <mergeCell ref="R3:AG3"/>
+    <mergeCell ref="AX2:BM2"/>
+    <mergeCell ref="BN2:CC2"/>
+    <mergeCell ref="CD2:CS2"/>
+    <mergeCell ref="CT2:DI2"/>
+    <mergeCell ref="DJ2:DY2"/>
+    <mergeCell ref="HB2:HQ2"/>
+    <mergeCell ref="HR2:IG2"/>
+    <mergeCell ref="IH2:IW2"/>
+    <mergeCell ref="DZ2:EO2"/>
+    <mergeCell ref="EP2:FE2"/>
+    <mergeCell ref="FF2:FU2"/>
+    <mergeCell ref="FV2:GK2"/>
+    <mergeCell ref="GL2:HA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>